<commit_message>
rerun figs and tables with corrected july teamster tp data
</commit_message>
<xml_diff>
--- a/Data/Correlation_matrices/Multivariable_correlation_matrix.xlsx
+++ b/Data/Correlation_matrices/Multivariable_correlation_matrix.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\immcc\Documents\SplashNBurn\Data\Correlation_matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{959351D9-B3EB-40F1-8BC9-82FF592306DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9591E467-7466-4EAF-A201-E6A5BAFC657D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TP_correlation_matrix" sheetId="1" r:id="rId1"/>
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -998,12 +998,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,22 +1089,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.23</v>
+        <v>0.05</v>
       </c>
       <c r="C4">
-        <v>-0.05</v>
+        <v>0.39</v>
       </c>
       <c r="D4">
-        <v>0.09</v>
+        <v>0.5</v>
       </c>
       <c r="E4">
-        <v>-0.1</v>
+        <v>0.32</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.46</v>
       </c>
       <c r="G4">
-        <v>0.11</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>